<commit_message>
refactor 5: KAF007: Add print
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF007_勤務変更申請\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02.Projects\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27270" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="勤務変更申請" sheetId="28" r:id="rId1"/>
@@ -58,30 +58,24 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -102,7 +96,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -320,7 +314,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -462,9 +456,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -495,13 +495,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>30291</xdr:colOff>
+      <xdr:colOff>1716</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>643207</xdr:colOff>
+      <xdr:colOff>614632</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>174130</xdr:rowOff>
     </xdr:to>
@@ -510,7 +510,7 @@
         <xdr:cNvPr id="65" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -518,8 +518,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3440241" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="2821116" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -529,7 +529,7 @@
           <xdr:cNvPr id="66" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -583,7 +583,7 @@
           <xdr:cNvPr id="67" name="直線コネクタ 66">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -623,7 +623,7 @@
           <xdr:cNvPr id="68" name="直線コネクタ 67">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -663,7 +663,7 @@
           <xdr:cNvPr id="69" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -701,13 +701,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -716,7 +719,7 @@
           <xdr:cNvPr id="70" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -754,13 +757,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -769,7 +775,7 @@
           <xdr:cNvPr id="71" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -807,13 +813,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -822,14 +831,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>27688</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>618238</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>640604</xdr:colOff>
+      <xdr:colOff>612029</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>174130</xdr:rowOff>
     </xdr:to>
@@ -838,7 +847,7 @@
         <xdr:cNvPr id="72" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -846,8 +855,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4104388" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3370963" y="223630"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -857,7 +866,7 @@
           <xdr:cNvPr id="73" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -911,7 +920,7 @@
           <xdr:cNvPr id="74" name="直線コネクタ 73">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -951,7 +960,7 @@
           <xdr:cNvPr id="75" name="直線コネクタ 74">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -991,7 +1000,7 @@
           <xdr:cNvPr id="76" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1029,13 +1038,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1044,7 +1056,7 @@
           <xdr:cNvPr id="77" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1082,13 +1094,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1097,7 +1112,7 @@
           <xdr:cNvPr id="78" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1135,13 +1150,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1151,13 +1169,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>33131</xdr:colOff>
+      <xdr:colOff>4556</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>646047</xdr:colOff>
+      <xdr:colOff>617472</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>174130</xdr:rowOff>
     </xdr:to>
@@ -1166,7 +1184,7 @@
         <xdr:cNvPr id="79" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1174,8 +1192,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4776581" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3928856" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1185,7 +1203,7 @@
           <xdr:cNvPr id="80" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1239,7 +1257,7 @@
           <xdr:cNvPr id="81" name="直線コネクタ 80">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1279,7 +1297,7 @@
           <xdr:cNvPr id="82" name="直線コネクタ 81">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1319,7 +1337,7 @@
           <xdr:cNvPr id="83" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1357,13 +1375,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1372,7 +1393,7 @@
           <xdr:cNvPr id="84" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1410,13 +1431,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1425,7 +1449,7 @@
           <xdr:cNvPr id="85" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1463,13 +1487,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1478,14 +1505,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>27689</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>618239</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>640605</xdr:colOff>
+      <xdr:colOff>612030</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>174130</xdr:rowOff>
     </xdr:to>
@@ -1494,7 +1521,7 @@
         <xdr:cNvPr id="86" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1502,8 +1529,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5437889" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="4475864" y="223630"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1513,7 +1540,7 @@
           <xdr:cNvPr id="87" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1567,7 +1594,7 @@
           <xdr:cNvPr id="88" name="直線コネクタ 87">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1607,7 +1634,7 @@
           <xdr:cNvPr id="89" name="直線コネクタ 88">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1647,7 +1674,7 @@
           <xdr:cNvPr id="90" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1685,13 +1712,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1700,7 +1730,7 @@
           <xdr:cNvPr id="91" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1738,13 +1768,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1753,7 +1786,7 @@
           <xdr:cNvPr id="92" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1791,13 +1824,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1807,13 +1843,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>33132</xdr:colOff>
+      <xdr:colOff>4557</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>646048</xdr:colOff>
+      <xdr:colOff>617473</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>174130</xdr:rowOff>
     </xdr:to>
@@ -1822,7 +1858,7 @@
         <xdr:cNvPr id="93" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1830,8 +1866,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6110082" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="5033757" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1841,7 +1877,7 @@
           <xdr:cNvPr id="94" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1895,7 +1931,7 @@
           <xdr:cNvPr id="95" name="直線コネクタ 94">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1935,7 +1971,7 @@
           <xdr:cNvPr id="96" name="直線コネクタ 95">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1975,7 +2011,7 @@
           <xdr:cNvPr id="97" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2013,13 +2049,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2028,7 +2067,7 @@
           <xdr:cNvPr id="98" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2066,13 +2105,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2081,7 +2123,7 @@
           <xdr:cNvPr id="99" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2119,13 +2161,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2523,20 +2568,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.88671875" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.88671875" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.44140625" style="2"/>
+    <col min="18" max="16384" width="2.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2601,8 +2646,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -2615,8 +2660,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -2632,11 +2677,11 @@
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="17"/>
       <c r="L8" s="1"/>
@@ -2645,14 +2690,14 @@
       <c r="A9" s="1"/>
       <c r="B9" s="35"/>
       <c r="C9" s="36"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
@@ -2660,11 +2705,11 @@
       <c r="B10" s="35"/>
       <c r="C10" s="36"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="17"/>
       <c r="L10" s="1"/>
@@ -2673,20 +2718,20 @@
       <c r="A11" s="1"/>
       <c r="B11" s="35"/>
       <c r="C11" s="36"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="14"/>
       <c r="E12" s="15"/>
       <c r="F12" s="16"/>
@@ -2699,16 +2744,16 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="3.75" customHeight="1">
@@ -2725,7 +2770,7 @@
       <c r="K14" s="22"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="63.75" customHeight="1">
+    <row r="15" spans="1:12" ht="90" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="37"/>
       <c r="C15" s="38"/>
@@ -2987,7 +3032,7 @@
     <row r="41" spans="2:11" ht="15" customHeight="1"/>
     <row r="42" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="10">
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="B18:C18"/>
@@ -2995,15 +3040,12 @@
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
refactor 5: KAF007: fix Update ly do man B
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02.Projects\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF007_勤務変更申請\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27270" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="勤務変更申請" sheetId="28" r:id="rId1"/>
@@ -701,16 +701,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -757,16 +754,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -821,7 +815,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>   </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1038,16 +1032,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1094,16 +1085,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1158,7 +1146,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>  </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1375,16 +1363,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1431,16 +1416,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1495,7 +1477,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>  </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1712,16 +1694,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1768,16 +1747,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1832,7 +1808,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>  </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -2049,16 +2025,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2105,16 +2078,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2169,7 +2139,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>  </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -2569,7 +2539,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
refactor 5: KAF007: Update enable mode chi tiet
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
@@ -701,6 +701,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -754,13 +764,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -815,7 +828,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>   </a:t>
+              <a:t>    </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1032,13 +1045,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t>  </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1085,13 +1101,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1146,7 +1165,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t>    </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1363,13 +1382,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t>  </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1416,13 +1438,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1477,7 +1502,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t>   </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1694,13 +1719,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t>  </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1747,13 +1775,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1808,7 +1839,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t>   </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -2025,13 +2056,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2078,13 +2112,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2139,7 +2176,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t>   </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -2539,7 +2576,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
refactor 5: KAF007: Update Ui
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
@@ -510,7 +510,7 @@
         <xdr:cNvPr id="65" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -529,7 +529,7 @@
           <xdr:cNvPr id="66" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -583,7 +583,7 @@
           <xdr:cNvPr id="67" name="直線コネクタ 66">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -623,7 +623,7 @@
           <xdr:cNvPr id="68" name="直線コネクタ 67">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -663,7 +663,7 @@
           <xdr:cNvPr id="69" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -726,7 +726,7 @@
           <xdr:cNvPr id="70" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -782,7 +782,7 @@
           <xdr:cNvPr id="71" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -854,7 +854,7 @@
         <xdr:cNvPr id="72" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,7 +873,7 @@
           <xdr:cNvPr id="73" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -927,7 +927,7 @@
           <xdr:cNvPr id="74" name="直線コネクタ 73">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -967,7 +967,7 @@
           <xdr:cNvPr id="75" name="直線コネクタ 74">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1007,7 +1007,7 @@
           <xdr:cNvPr id="76" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1063,7 +1063,7 @@
           <xdr:cNvPr id="77" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1119,7 +1119,7 @@
           <xdr:cNvPr id="78" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1191,7 +1191,7 @@
         <xdr:cNvPr id="79" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1210,7 +1210,7 @@
           <xdr:cNvPr id="80" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1264,7 +1264,7 @@
           <xdr:cNvPr id="81" name="直線コネクタ 80">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1304,7 +1304,7 @@
           <xdr:cNvPr id="82" name="直線コネクタ 81">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1344,7 +1344,7 @@
           <xdr:cNvPr id="83" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1390,7 +1390,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1400,7 +1400,7 @@
           <xdr:cNvPr id="84" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1456,7 +1456,7 @@
           <xdr:cNvPr id="85" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1528,7 +1528,7 @@
         <xdr:cNvPr id="86" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1547,7 +1547,7 @@
           <xdr:cNvPr id="87" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1601,7 +1601,7 @@
           <xdr:cNvPr id="88" name="直線コネクタ 87">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1641,7 +1641,7 @@
           <xdr:cNvPr id="89" name="直線コネクタ 88">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1681,7 +1681,7 @@
           <xdr:cNvPr id="90" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1727,7 +1727,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1737,7 +1737,7 @@
           <xdr:cNvPr id="91" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1793,7 +1793,7 @@
           <xdr:cNvPr id="92" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1865,7 +1865,7 @@
         <xdr:cNvPr id="93" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1884,7 +1884,7 @@
           <xdr:cNvPr id="94" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1938,7 +1938,7 @@
           <xdr:cNvPr id="95" name="直線コネクタ 94">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1978,7 +1978,7 @@
           <xdr:cNvPr id="96" name="直線コネクタ 95">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2018,7 +2018,7 @@
           <xdr:cNvPr id="97" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2074,7 +2074,7 @@
           <xdr:cNvPr id="98" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2130,7 +2130,7 @@
           <xdr:cNvPr id="99" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2576,7 +2576,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
refactor 5: KAF007: Update tempalte file in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
@@ -510,7 +510,7 @@
         <xdr:cNvPr id="65" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -529,7 +529,7 @@
           <xdr:cNvPr id="66" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -583,7 +583,7 @@
           <xdr:cNvPr id="67" name="直線コネクタ 66">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -623,7 +623,7 @@
           <xdr:cNvPr id="68" name="直線コネクタ 67">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -663,7 +663,7 @@
           <xdr:cNvPr id="69" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -726,7 +726,7 @@
           <xdr:cNvPr id="70" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -782,7 +782,7 @@
           <xdr:cNvPr id="71" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -854,7 +854,7 @@
         <xdr:cNvPr id="72" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,7 +873,7 @@
           <xdr:cNvPr id="73" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -927,7 +927,7 @@
           <xdr:cNvPr id="74" name="直線コネクタ 73">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -967,7 +967,7 @@
           <xdr:cNvPr id="75" name="直線コネクタ 74">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1007,7 +1007,7 @@
           <xdr:cNvPr id="76" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1053,7 +1053,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>  </a:t>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1063,7 +1063,7 @@
           <xdr:cNvPr id="77" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1119,7 +1119,7 @@
           <xdr:cNvPr id="78" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1191,7 +1191,7 @@
         <xdr:cNvPr id="79" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1210,7 +1210,7 @@
           <xdr:cNvPr id="80" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1264,7 +1264,7 @@
           <xdr:cNvPr id="81" name="直線コネクタ 80">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1304,7 +1304,7 @@
           <xdr:cNvPr id="82" name="直線コネクタ 81">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1344,7 +1344,7 @@
           <xdr:cNvPr id="83" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1400,7 +1400,7 @@
           <xdr:cNvPr id="84" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1456,7 +1456,7 @@
           <xdr:cNvPr id="85" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1528,7 +1528,7 @@
         <xdr:cNvPr id="86" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1547,7 +1547,7 @@
           <xdr:cNvPr id="87" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1601,7 +1601,7 @@
           <xdr:cNvPr id="88" name="直線コネクタ 87">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1641,7 +1641,7 @@
           <xdr:cNvPr id="89" name="直線コネクタ 88">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1681,7 +1681,7 @@
           <xdr:cNvPr id="90" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1737,7 +1737,7 @@
           <xdr:cNvPr id="91" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1793,7 +1793,7 @@
           <xdr:cNvPr id="92" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1865,7 +1865,7 @@
         <xdr:cNvPr id="93" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1884,7 +1884,7 @@
           <xdr:cNvPr id="94" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1938,7 +1938,7 @@
           <xdr:cNvPr id="95" name="直線コネクタ 94">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1978,7 +1978,7 @@
           <xdr:cNvPr id="96" name="直線コネクタ 95">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2018,7 +2018,7 @@
           <xdr:cNvPr id="97" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2074,7 +2074,7 @@
           <xdr:cNvPr id="98" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2130,7 +2130,7 @@
           <xdr:cNvPr id="99" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>

</xml_diff>

<commit_message>
refactor 5: KAF007: Update function in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF007_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27405" windowHeight="12825"/>
   </bookViews>
   <sheets>
     <sheet name="勤務変更申請" sheetId="28" r:id="rId1"/>
@@ -63,19 +63,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -96,7 +96,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -314,7 +314,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -420,51 +420,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -510,7 +501,7 @@
         <xdr:cNvPr id="65" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -518,8 +509,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2821116" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="3164016" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -529,7 +520,7 @@
           <xdr:cNvPr id="66" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -583,7 +574,7 @@
           <xdr:cNvPr id="67" name="直線コネクタ 66">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -623,7 +614,7 @@
           <xdr:cNvPr id="68" name="直線コネクタ 67">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -663,7 +654,7 @@
           <xdr:cNvPr id="69" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -726,7 +717,7 @@
           <xdr:cNvPr id="70" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -765,7 +756,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -774,6 +765,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -782,7 +780,7 @@
           <xdr:cNvPr id="71" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -821,15 +819,22 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>    </a:t>
+              <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -854,7 +859,7 @@
         <xdr:cNvPr id="72" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -862,8 +867,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3370963" y="223630"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3780538" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -873,7 +878,7 @@
           <xdr:cNvPr id="73" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -927,7 +932,7 @@
           <xdr:cNvPr id="74" name="直線コネクタ 73">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -967,7 +972,7 @@
           <xdr:cNvPr id="75" name="直線コネクタ 74">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1007,7 +1012,7 @@
           <xdr:cNvPr id="76" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1046,7 +1051,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1055,6 +1060,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1063,7 +1075,7 @@
           <xdr:cNvPr id="77" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1102,7 +1114,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1111,6 +1123,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1119,7 +1138,7 @@
           <xdr:cNvPr id="78" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1158,15 +1177,22 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>    </a:t>
+              <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1191,7 +1217,7 @@
         <xdr:cNvPr id="79" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1199,8 +1225,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3928856" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="4405106" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1210,7 +1236,7 @@
           <xdr:cNvPr id="80" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1264,7 +1290,7 @@
           <xdr:cNvPr id="81" name="直線コネクタ 80">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1304,7 +1330,7 @@
           <xdr:cNvPr id="82" name="直線コネクタ 81">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1344,7 +1370,7 @@
           <xdr:cNvPr id="83" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1383,7 +1409,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1392,6 +1418,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1400,7 +1433,7 @@
           <xdr:cNvPr id="84" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1439,7 +1472,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1448,6 +1481,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1456,7 +1496,7 @@
           <xdr:cNvPr id="85" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1495,15 +1535,22 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>   </a:t>
+              <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1528,7 +1575,7 @@
         <xdr:cNvPr id="86" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1536,8 +1583,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4475864" y="223630"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="5018789" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1547,7 +1594,7 @@
           <xdr:cNvPr id="87" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1601,7 +1648,7 @@
           <xdr:cNvPr id="88" name="直線コネクタ 87">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1641,7 +1688,7 @@
           <xdr:cNvPr id="89" name="直線コネクタ 88">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1681,7 +1728,7 @@
           <xdr:cNvPr id="90" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1720,7 +1767,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1729,6 +1776,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1737,7 +1791,7 @@
           <xdr:cNvPr id="91" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1776,7 +1830,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -1785,6 +1839,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1793,7 +1854,7 @@
           <xdr:cNvPr id="92" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1832,15 +1893,22 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>   </a:t>
+              <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1865,7 +1933,7 @@
         <xdr:cNvPr id="93" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1873,8 +1941,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5033757" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="5643357" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1884,7 +1952,7 @@
           <xdr:cNvPr id="94" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1938,7 +2006,7 @@
           <xdr:cNvPr id="95" name="直線コネクタ 94">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1978,7 +2046,7 @@
           <xdr:cNvPr id="96" name="直線コネクタ 95">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2018,7 +2086,7 @@
           <xdr:cNvPr id="97" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2064,7 +2132,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>  </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -2074,7 +2142,7 @@
           <xdr:cNvPr id="98" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2113,7 +2181,7 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -2122,6 +2190,13 @@
               </a:rPr>
               <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2130,7 +2205,7 @@
           <xdr:cNvPr id="99" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2169,15 +2244,22 @@
           <a:p>
             <a:pPr algn="ctr"/>
             <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t>   </a:t>
+              <a:t> </a:t>
             </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2576,19 +2658,19 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.5" style="2"/>
+    <col min="18" max="16384" width="2.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2612,10 +2694,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -2626,10 +2708,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -2653,8 +2735,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -2667,8 +2749,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -2681,8 +2763,8 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="14"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -2695,8 +2777,8 @@
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="14"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -2709,8 +2791,8 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="14"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -2723,8 +2805,8 @@
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="14"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -2737,8 +2819,8 @@
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="14"/>
       <c r="E12" s="15"/>
       <c r="F12" s="16"/>
@@ -2751,8 +2833,8 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
@@ -2779,16 +2861,16 @@
     </row>
     <row r="15" spans="1:12" ht="90" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="3.75" customHeight="1">
@@ -2821,16 +2903,16 @@
     </row>
     <row r="18" spans="1:12" ht="74.25" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="44"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="3.75" customHeight="1">
@@ -3039,7 +3121,7 @@
     <row r="41" spans="2:11" ht="15" customHeight="1"/>
     <row r="42" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="B18:C18"/>
@@ -3050,6 +3132,10 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>